<commit_message>
yandex fix + begin minor ui restructuring
</commit_message>
<xml_diff>
--- a/vedsite/generated/36a70659-5556-4ee6-ad66-f87e39e3d8be/211/tablecache.xlsx
+++ b/vedsite/generated/36a70659-5556-4ee6-ad66-f87e39e3d8be/211/tablecache.xlsx
@@ -9,7 +9,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191029" fullCalcOnLoad="1"/>
+  <calcPr calcId="179021" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -170,30 +170,14 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center"/>
     </xf>
@@ -209,6 +193,23 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -592,622 +593,622 @@
   <dimension ref="A1:AB7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B7" sqref="B4:B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="18" customWidth="1" min="1" max="1"/>
-    <col width="18.44140625" customWidth="1" min="2" max="2"/>
-    <col width="9.109375" customWidth="1" min="12" max="12"/>
+    <col width="18.42578125" customWidth="1" min="2" max="2"/>
+    <col width="9.140625" customWidth="1" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21" customHeight="1">
+    <row r="1" ht="20.25" customHeight="1">
       <c r="A1" s="1" t="n"/>
       <c r="B1" s="1" t="n"/>
-      <c r="C1" s="6" t="inlineStr">
+      <c r="C1" s="15" t="inlineStr">
         <is>
           <t>Yandex</t>
         </is>
       </c>
-      <c r="D1" s="3" t="n"/>
-      <c r="E1" s="3" t="n"/>
-      <c r="F1" s="3" t="n"/>
-      <c r="G1" s="3" t="n"/>
-      <c r="H1" s="3" t="n"/>
-      <c r="I1" s="3" t="n"/>
-      <c r="J1" s="3" t="n"/>
-      <c r="K1" s="3" t="n"/>
-      <c r="L1" s="4" t="n"/>
-      <c r="M1" s="2" t="inlineStr">
+      <c r="D1" s="9" t="n"/>
+      <c r="E1" s="9" t="n"/>
+      <c r="F1" s="9" t="n"/>
+      <c r="G1" s="9" t="n"/>
+      <c r="H1" s="9" t="n"/>
+      <c r="I1" s="9" t="n"/>
+      <c r="J1" s="9" t="n"/>
+      <c r="K1" s="9" t="n"/>
+      <c r="L1" s="10" t="n"/>
+      <c r="M1" s="8" t="inlineStr">
         <is>
           <t>Stepik</t>
         </is>
       </c>
-      <c r="N1" s="3" t="n"/>
-      <c r="O1" s="4" t="n"/>
-      <c r="P1" s="5" t="inlineStr">
+      <c r="N1" s="9" t="n"/>
+      <c r="O1" s="10" t="n"/>
+      <c r="P1" s="14" t="inlineStr">
         <is>
           <t>Yandex</t>
         </is>
       </c>
-      <c r="Q1" s="3" t="n"/>
-      <c r="R1" s="3" t="n"/>
-      <c r="S1" s="3" t="n"/>
-      <c r="T1" s="3" t="n"/>
-      <c r="U1" s="3" t="n"/>
-      <c r="V1" s="3" t="n"/>
-      <c r="W1" s="3" t="n"/>
-      <c r="X1" s="3" t="n"/>
-      <c r="Y1" s="4" t="n"/>
-      <c r="Z1" s="2" t="inlineStr">
+      <c r="Q1" s="9" t="n"/>
+      <c r="R1" s="9" t="n"/>
+      <c r="S1" s="9" t="n"/>
+      <c r="T1" s="9" t="n"/>
+      <c r="U1" s="9" t="n"/>
+      <c r="V1" s="9" t="n"/>
+      <c r="W1" s="9" t="n"/>
+      <c r="X1" s="9" t="n"/>
+      <c r="Y1" s="10" t="n"/>
+      <c r="Z1" s="8" t="inlineStr">
         <is>
           <t>Stepik</t>
         </is>
       </c>
-      <c r="AA1" s="3" t="n"/>
-      <c r="AB1" s="4" t="n"/>
+      <c r="AA1" s="9" t="n"/>
+      <c r="AB1" s="10" t="n"/>
     </row>
-    <row r="2" ht="15.6" customHeight="1">
-      <c r="A2" s="8" t="n"/>
-      <c r="B2" s="8" t="n"/>
-      <c r="C2" s="8" t="inlineStr">
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="11" t="n"/>
+      <c r="B2" s="11" t="n"/>
+      <c r="C2" s="11" t="inlineStr">
         <is>
           <t>Contest 1234</t>
         </is>
       </c>
-      <c r="D2" s="3" t="n"/>
-      <c r="E2" s="3" t="n"/>
-      <c r="F2" s="3" t="n"/>
-      <c r="G2" s="3" t="n"/>
-      <c r="H2" s="3" t="n"/>
-      <c r="I2" s="3" t="n"/>
-      <c r="J2" s="3" t="n"/>
-      <c r="K2" s="3" t="n"/>
-      <c r="L2" s="4" t="n"/>
-      <c r="M2" s="8" t="inlineStr">
+      <c r="D2" s="9" t="n"/>
+      <c r="E2" s="9" t="n"/>
+      <c r="F2" s="9" t="n"/>
+      <c r="G2" s="9" t="n"/>
+      <c r="H2" s="9" t="n"/>
+      <c r="I2" s="9" t="n"/>
+      <c r="J2" s="9" t="n"/>
+      <c r="K2" s="9" t="n"/>
+      <c r="L2" s="10" t="n"/>
+      <c r="M2" s="11" t="inlineStr">
         <is>
           <t>Contest 2345</t>
         </is>
       </c>
-      <c r="N2" s="3" t="n"/>
-      <c r="O2" s="4" t="n"/>
-      <c r="P2" s="8" t="inlineStr">
+      <c r="N2" s="9" t="n"/>
+      <c r="O2" s="10" t="n"/>
+      <c r="P2" s="11" t="inlineStr">
         <is>
           <t>Contest 1234</t>
         </is>
       </c>
-      <c r="Q2" s="3" t="n"/>
-      <c r="R2" s="3" t="n"/>
-      <c r="S2" s="3" t="n"/>
-      <c r="T2" s="3" t="n"/>
-      <c r="U2" s="3" t="n"/>
-      <c r="V2" s="3" t="n"/>
-      <c r="W2" s="3" t="n"/>
-      <c r="X2" s="3" t="n"/>
-      <c r="Y2" s="4" t="n"/>
-      <c r="Z2" s="8" t="inlineStr">
+      <c r="Q2" s="9" t="n"/>
+      <c r="R2" s="9" t="n"/>
+      <c r="S2" s="9" t="n"/>
+      <c r="T2" s="9" t="n"/>
+      <c r="U2" s="9" t="n"/>
+      <c r="V2" s="9" t="n"/>
+      <c r="W2" s="9" t="n"/>
+      <c r="X2" s="9" t="n"/>
+      <c r="Y2" s="10" t="n"/>
+      <c r="Z2" s="11" t="inlineStr">
         <is>
           <t>Contest 2345</t>
         </is>
       </c>
-      <c r="AA2" s="3" t="n"/>
-      <c r="AB2" s="4" t="n"/>
+      <c r="AA2" s="9" t="n"/>
+      <c r="AB2" s="10" t="n"/>
     </row>
-    <row r="3" ht="15.6" customHeight="1">
-      <c r="A3" s="8" t="inlineStr">
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="11" t="inlineStr">
         <is>
           <t>Student</t>
         </is>
       </c>
-      <c r="B3" s="8" t="inlineStr">
+      <c r="B3" s="11" t="inlineStr">
         <is>
           <t>Student email</t>
         </is>
       </c>
-      <c r="C3" s="8" t="inlineStr">
+      <c r="C3" s="11" t="inlineStr">
         <is>
           <t>Task 1</t>
         </is>
       </c>
-      <c r="D3" s="8" t="inlineStr">
+      <c r="D3" s="11" t="inlineStr">
         <is>
           <t>Task 2</t>
         </is>
       </c>
-      <c r="E3" s="8" t="inlineStr">
+      <c r="E3" s="11" t="inlineStr">
         <is>
           <t>Task 3</t>
         </is>
       </c>
-      <c r="F3" s="8" t="inlineStr">
+      <c r="F3" s="11" t="inlineStr">
         <is>
           <t>Task 4</t>
         </is>
       </c>
-      <c r="G3" s="8" t="inlineStr">
+      <c r="G3" s="11" t="inlineStr">
         <is>
           <t>Task 5</t>
         </is>
       </c>
-      <c r="H3" s="8" t="inlineStr">
+      <c r="H3" s="11" t="inlineStr">
         <is>
           <t>Task 6</t>
         </is>
       </c>
-      <c r="I3" s="8" t="inlineStr">
+      <c r="I3" s="11" t="inlineStr">
         <is>
           <t>Task 7</t>
         </is>
       </c>
-      <c r="J3" s="8" t="inlineStr">
+      <c r="J3" s="11" t="inlineStr">
         <is>
           <t>Task 8</t>
         </is>
       </c>
-      <c r="K3" s="8" t="inlineStr">
+      <c r="K3" s="11" t="inlineStr">
         <is>
           <t>Task 9</t>
         </is>
       </c>
-      <c r="L3" s="8" t="inlineStr">
+      <c r="L3" s="11" t="inlineStr">
         <is>
           <t>Sum</t>
         </is>
       </c>
-      <c r="M3" s="8" t="inlineStr">
+      <c r="M3" s="11" t="inlineStr">
         <is>
           <t>Task 1</t>
         </is>
       </c>
-      <c r="N3" s="8" t="inlineStr">
+      <c r="N3" s="11" t="inlineStr">
         <is>
           <t>Task 2</t>
         </is>
       </c>
-      <c r="O3" s="8" t="inlineStr">
+      <c r="O3" s="11" t="inlineStr">
         <is>
           <t>Sum</t>
         </is>
       </c>
-      <c r="P3" s="8" t="inlineStr">
+      <c r="P3" s="11" t="inlineStr">
         <is>
           <t>Task 1</t>
         </is>
       </c>
-      <c r="Q3" s="8" t="inlineStr">
+      <c r="Q3" s="11" t="inlineStr">
         <is>
           <t>Task 2</t>
         </is>
       </c>
-      <c r="R3" s="8" t="inlineStr">
+      <c r="R3" s="11" t="inlineStr">
         <is>
           <t>Task 3</t>
         </is>
       </c>
-      <c r="S3" s="8" t="inlineStr">
+      <c r="S3" s="11" t="inlineStr">
         <is>
           <t>Task 4</t>
         </is>
       </c>
-      <c r="T3" s="8" t="inlineStr">
+      <c r="T3" s="11" t="inlineStr">
         <is>
           <t>Task 5</t>
         </is>
       </c>
-      <c r="U3" s="8" t="inlineStr">
+      <c r="U3" s="11" t="inlineStr">
         <is>
           <t>Task 6</t>
         </is>
       </c>
-      <c r="V3" s="8" t="inlineStr">
+      <c r="V3" s="11" t="inlineStr">
         <is>
           <t>Task 7</t>
         </is>
       </c>
-      <c r="W3" s="8" t="inlineStr">
+      <c r="W3" s="11" t="inlineStr">
         <is>
           <t>Task 8</t>
         </is>
       </c>
-      <c r="X3" s="8" t="inlineStr">
+      <c r="X3" s="11" t="inlineStr">
         <is>
           <t>Task 9</t>
         </is>
       </c>
-      <c r="Y3" s="8" t="inlineStr">
+      <c r="Y3" s="11" t="inlineStr">
         <is>
           <t>Sum</t>
         </is>
       </c>
-      <c r="Z3" s="8" t="inlineStr">
+      <c r="Z3" s="11" t="inlineStr">
         <is>
           <t>Task 1</t>
         </is>
       </c>
-      <c r="AA3" s="8" t="inlineStr">
+      <c r="AA3" s="11" t="inlineStr">
         <is>
           <t>Task 2</t>
         </is>
       </c>
-      <c r="AB3" s="8" t="inlineStr">
+      <c r="AB3" s="11" t="inlineStr">
         <is>
           <t>Sum</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="15.6" customHeight="1">
-      <c r="A4" s="8" t="inlineStr">
-        <is>
-          <t>Вася Пупкин</t>
-        </is>
-      </c>
-      <c r="B4" s="11" t="inlineStr">
-        <is>
-          <t>xoxo@gmail.com</t>
-        </is>
-      </c>
-      <c r="C4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" s="8" t="n">
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="11" t="inlineStr">
+        <is>
+          <t>Василий Раневский</t>
+        </is>
+      </c>
+      <c r="B4" s="16" t="inlineStr">
+        <is>
+          <t>valisius@gmail.com</t>
+        </is>
+      </c>
+      <c r="C4" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="M4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="N4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="P4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="R4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="S4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="U4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="V4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="W4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="X4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="8" t="n">
+      <c r="M4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N4" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="P4" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="R4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="S4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="T4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="U4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="V4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="W4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="X4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="Z4" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="8" t="n">
+      <c r="Z4" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="11" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="5" ht="15.6" customHeight="1">
-      <c r="A5" s="8" t="inlineStr">
-        <is>
-          <t>Лол Кек</t>
-        </is>
-      </c>
-      <c r="B5" s="11" t="inlineStr">
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="11" t="inlineStr">
+        <is>
+          <t>Александр Пушной</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
         <is>
           <t>lolkek@edu.hse.ru</t>
         </is>
       </c>
-      <c r="C5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="O5" s="8" t="n">
+      <c r="C5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="O5" s="11" t="n">
         <v>2</v>
       </c>
-      <c r="P5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="U5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="V5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="W5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="X5" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="Z5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA5" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="8" t="n">
+      <c r="P5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="W5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X5" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="11" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="6" ht="15.6" customHeight="1">
-      <c r="A6" s="8" t="inlineStr">
-        <is>
-          <t>Памагите Пажождаааа</t>
-        </is>
-      </c>
-      <c r="B6" s="11" t="inlineStr">
-        <is>
-          <t>pomogite@mail.ru</t>
-        </is>
-      </c>
-      <c r="C6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L6" s="8" t="n">
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="11" t="inlineStr">
+        <is>
+          <t>Евгений Рабочев</t>
+        </is>
+      </c>
+      <c r="B6" s="16" t="inlineStr">
+        <is>
+          <t>evgeniy.rabochev.2000@mail.ru</t>
+        </is>
+      </c>
+      <c r="C6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L6" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="M6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="N6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="P6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="T6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="U6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="V6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="W6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="X6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="8" t="n">
+      <c r="M6" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="N6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O6" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="P6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="T6" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="U6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="V6" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="W6" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="X6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="Z6" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="8" t="n">
+      <c r="Z6" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="11" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="7" ht="15.6" customHeight="1">
-      <c r="A7" s="8" t="inlineStr">
-        <is>
-          <t>Никто Никитов</t>
-        </is>
-      </c>
-      <c r="B7" s="11" t="inlineStr">
-        <is>
-          <t>nope@nope.nope</t>
-        </is>
-      </c>
-      <c r="C7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="N7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="O7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="P7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="R7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="S7" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="T7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="U7" s="8" t="n">
-        <v>1</v>
-      </c>
-      <c r="V7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="W7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="X7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="8" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="8" t="n">
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="11" t="inlineStr">
+        <is>
+          <t>Никита Никитов</t>
+        </is>
+      </c>
+      <c r="B7" s="16" t="inlineStr">
+        <is>
+          <t>nope@nope.com</t>
+        </is>
+      </c>
+      <c r="C7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="L7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="M7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="O7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="P7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="R7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="S7" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="T7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="U7" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="V7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="W7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="X7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="11" t="n">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="11" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="8" ht="15.6" customHeight="1"/>
-    <row r="9" ht="15.6" customHeight="1"/>
-    <row r="10" ht="15.6" customHeight="1"/>
-    <row r="11" ht="15.6" customHeight="1"/>
-    <row r="12" ht="15.6" customHeight="1"/>
-    <row r="13" ht="15.6" customHeight="1"/>
-    <row r="14" ht="15.6" customHeight="1"/>
-    <row r="15" ht="15.6" customHeight="1"/>
-    <row r="16" ht="15.6" customHeight="1"/>
-    <row r="17" ht="15.6" customHeight="1"/>
-    <row r="18" ht="15.6" customHeight="1"/>
-    <row r="19" ht="15.6" customHeight="1"/>
+    <row r="8" ht="15.75" customHeight="1"/>
+    <row r="9" ht="15.75" customHeight="1"/>
+    <row r="10" ht="15.75" customHeight="1"/>
+    <row r="11" ht="15.75" customHeight="1"/>
+    <row r="12" ht="15.75" customHeight="1"/>
+    <row r="13" ht="15.75" customHeight="1"/>
+    <row r="14" ht="15.75" customHeight="1"/>
+    <row r="15" ht="15.75" customHeight="1"/>
+    <row r="16" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1"/>
+    <row r="18" ht="15.75" customHeight="1"/>
+    <row r="19" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="8">
     <mergeCell ref="Z1:AB1"/>

</xml_diff>